<commit_message>
Fixing some imports and updating authorizartion
</commit_message>
<xml_diff>
--- a/cohort-engine-api-web/src/test/resources/2.16.840.1.113762.1.4.1114.7.xlsx
+++ b/cohort-engine-api-web/src/test/resources/2.16.840.1.113762.1.4.1114.7.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mshelley/Documents/weirdStuff/quality-measure-and-cohort-service/fhir-resource-tooling/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mshelley/Documents/weirdStuff/quality-measure-and-cohort-service/cohort-engine-api-web/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C298BA4A-D9D4-EE42-A30D-68459E262962}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F65AB29-90A7-A841-B8CE-839E47D6A56D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,19 +40,10 @@
     <t>Value Set Name</t>
   </si>
   <si>
-    <t>2019 Novel Coronavirus COVID 19 Codeset</t>
-  </si>
-  <si>
     <t>Code System</t>
   </si>
   <si>
     <t>SNOMEDCT</t>
-  </si>
-  <si>
-    <t>OID</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113762.1.4.1114.7</t>
   </si>
   <si>
     <t>Type</t>
@@ -201,6 +192,15 @@
   </si>
   <si>
     <t>Exposure to Severe acute respiratory syndrome coronavirus 2 (event)</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>testValueSet</t>
+  </si>
+  <si>
+    <t>Value Set For Testing Uploads</t>
   </si>
 </sst>
 </file>
@@ -384,6 +384,50 @@
         <a:xfrm>
           <a:off x="0" y="0"/>
           <a:ext cx="3838575" cy="552450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1170927</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Picture">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71ABE0A1-E270-B440-BEDD-B8EEF29B0A7D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="4218927" cy="3810"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -698,7 +742,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -714,90 +758,90 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:2" ht="80" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -817,7 +861,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -834,305 +878,305 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding wrappers around a few exceptions that get thrown to rethrow with more intelligible messages
</commit_message>
<xml_diff>
--- a/cohort-engine-api-web/src/test/resources/2.16.840.1.113762.1.4.1114.7.xlsx
+++ b/cohort-engine-api-web/src/test/resources/2.16.840.1.113762.1.4.1114.7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mshelley/Documents/weirdStuff/quality-measure-and-cohort-service/cohort-engine-api-web/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F65AB29-90A7-A841-B8CE-839E47D6A56D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42FCDE7-872D-D24C-B470-46B87704725D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -861,7 +861,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>